<commit_message>
V0 - Resultados Random Forest
</commit_message>
<xml_diff>
--- a/resultadosPrevisoes.xlsx
+++ b/resultadosPrevisoes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/Dissertacao2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D516BBC-F404-F349-A71F-13DEA9511E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAFEAF7-088F-B141-A15F-FEB77CA0E8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" activeTab="1" xr2:uid="{96FF22BC-28B8-9948-8104-5312DD65AA32}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{96FF22BC-28B8-9948-8104-5312DD65AA32}"/>
   </bookViews>
   <sheets>
-    <sheet name="Random Forest" sheetId="1" r:id="rId1"/>
-    <sheet name="Logistic Regression" sheetId="2" r:id="rId2"/>
+    <sheet name="RF_SelectKBest" sheetId="1" r:id="rId1"/>
+    <sheet name="FS_ " sheetId="3" r:id="rId2"/>
+    <sheet name="Logistic Regression" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -391,6 +392,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369D4BD9-9325-C34C-8095-2F214F4DDD53}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85126F1-0D46-2249-9FB3-EF18741CFBAF}">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -399,11 +412,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E27495-191A-4745-BA55-73F4B2776943}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>

</xml_diff>